<commit_message>
adding pairwise estimation, etc
</commit_message>
<xml_diff>
--- a/trends/temp/table2.xlsx
+++ b/trends/temp/table2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>year range</t>
   </si>
@@ -28,7 +28,61 @@
     <t>proportion drinking</t>
   </si>
   <si>
-    <t>(nan)</t>
+    <t>(0.21)</t>
+  </si>
+  <si>
+    <t>(0.63)</t>
+  </si>
+  <si>
+    <t>(0.32)</t>
+  </si>
+  <si>
+    <t>(0.31)</t>
+  </si>
+  <si>
+    <t>(0.11)</t>
+  </si>
+  <si>
+    <t>(0.43)</t>
+  </si>
+  <si>
+    <t>(1.08)</t>
+  </si>
+  <si>
+    <t>(0.22)</t>
+  </si>
+  <si>
+    <t>(0.48)</t>
+  </si>
+  <si>
+    <t>(0.23)</t>
+  </si>
+  <si>
+    <t>(0.53)</t>
+  </si>
+  <si>
+    <t>(0.77)</t>
+  </si>
+  <si>
+    <t>(0.00576)</t>
+  </si>
+  <si>
+    <t>(0.01094)</t>
+  </si>
+  <si>
+    <t>(0.00371)</t>
+  </si>
+  <si>
+    <t>(0.00413)</t>
+  </si>
+  <si>
+    <t>(0.00314)</t>
+  </si>
+  <si>
+    <t>(0.00709)</t>
+  </si>
+  <si>
+    <t>(0.01640)</t>
   </si>
 </sst>
 </file>
@@ -414,13 +468,13 @@
         <v>1983</v>
       </c>
       <c r="C2">
-        <v>7.57</v>
+        <v>7.5</v>
       </c>
       <c r="D2">
-        <v>6.91</v>
+        <v>6.89</v>
       </c>
       <c r="E2">
-        <v>0.267448</v>
+        <v>0.26759</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -434,10 +488,10 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -448,13 +502,13 @@
         <v>1988</v>
       </c>
       <c r="C4">
-        <v>7.96</v>
+        <v>8</v>
       </c>
       <c r="D4">
-        <v>7.84</v>
+        <v>7.9</v>
       </c>
       <c r="E4">
-        <v>0.217327</v>
+        <v>0.216508</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -465,13 +519,13 @@
         <v>1992</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -482,13 +536,13 @@
         <v>1993</v>
       </c>
       <c r="C6">
-        <v>8.41</v>
+        <v>8.32</v>
       </c>
       <c r="D6">
-        <v>8.57</v>
+        <v>8.5</v>
       </c>
       <c r="E6">
-        <v>0.166032</v>
+        <v>0.167751</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -499,13 +553,13 @@
         <v>1997</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D7" t="s">
         <v>4</v>
       </c>
       <c r="E7" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -516,13 +570,13 @@
         <v>1998</v>
       </c>
       <c r="C8">
-        <v>7.8</v>
+        <v>7.64</v>
       </c>
       <c r="D8">
-        <v>8.76</v>
+        <v>8.619999999999999</v>
       </c>
       <c r="E8">
-        <v>0.158294</v>
+        <v>0.161213</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -533,13 +587,13 @@
         <v>2002</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -550,13 +604,13 @@
         <v>2003</v>
       </c>
       <c r="C10">
-        <v>7.74</v>
+        <v>7.95</v>
       </c>
       <c r="D10">
-        <v>9.06</v>
+        <v>9.23</v>
       </c>
       <c r="E10">
-        <v>0.152469</v>
+        <v>0.149439</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -567,13 +621,13 @@
         <v>2007</v>
       </c>
       <c r="C11" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E11" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -584,13 +638,13 @@
         <v>2008</v>
       </c>
       <c r="C12">
-        <v>8.609999999999999</v>
+        <v>8.98</v>
       </c>
       <c r="D12">
-        <v>9.210000000000001</v>
+        <v>9.52</v>
       </c>
       <c r="E12">
-        <v>0.14377</v>
+        <v>0.139979</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -601,13 +655,13 @@
         <v>2012</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -618,13 +672,13 @@
         <v>2013</v>
       </c>
       <c r="C14">
-        <v>7.03</v>
+        <v>6.8</v>
       </c>
       <c r="D14">
-        <v>6.62</v>
+        <v>6.52</v>
       </c>
       <c r="E14">
-        <v>0.154877</v>
+        <v>0.157687</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -635,13 +689,13 @@
         <v>2017</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="E15" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>